<commit_message>
added my name and project url in excel sheet
</commit_message>
<xml_diff>
--- a/Open Source task.xlsx
+++ b/Open Source task.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legion\Desktop\open-source\Security-Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\New folder (3)\Security-Taskkk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655120EA-671F-4435-B8F2-FC3A0DB523E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -54,13 +53,22 @@
   </si>
   <si>
     <t>السيد اسامه رجب السيد</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حبيبة رزق عدلي </t>
+  </si>
+  <si>
+    <t>habibarezk54@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/WalTeR-RE/Open-Source-Uni-Project.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,21 +465,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B88C28-23A0-4FB2-A45B-5BE272931FEB}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="1" max="1" width="46.4140625" customWidth="1"/>
     <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -491,12 +499,24 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A364EA89-B4FA-4322-9DA7-87C8CDF404AF}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{65319477-3938-45F9-8CEB-9746D877D7C0}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>